<commit_message>
data availability table formatting
</commit_message>
<xml_diff>
--- a/PIF_PAF/Documentation/data_availability_table.xlsx
+++ b/PIF_PAF/Documentation/data_availability_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/PAF/UK-cancer-trends/PIF_PAF/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/zoey_richards_icr_ac_uk/Documents/Git/UK-cancer-trends/PIF_PAF/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{AE0EE90C-8DC7-4F32-A791-CAFF1D351458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{089F87BC-A74B-4066-BE47-3AFD75C3B0E3}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{AE0EE90C-8DC7-4F32-A791-CAFF1D351458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76612B50-0D58-46B5-857C-0317A19B2F15}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{36D318F9-7DEA-4114-A153-04803E687D9D}"/>
+    <workbookView xWindow="30600" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{36D318F9-7DEA-4114-A153-04803E687D9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,16 +111,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -142,10 +134,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="8"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,46 +173,37 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <b/>
@@ -218,12 +215,183 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,24 +407,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F2DE9A8-E283-46AE-846D-EC8B592003B3}" name="Table1" displayName="Table1" ref="A1:L39" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F2DE9A8-E283-46AE-846D-EC8B592003B3}" name="Table1" displayName="Table1" ref="A1:L39" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
   <autoFilter ref="A1:L39" xr:uid="{7F2DE9A8-E283-46AE-846D-EC8B592003B3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F39">
     <sortCondition descending="1" ref="E1:E39"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{19F95E98-3538-4B7E-81F9-BDED2C5F55CB}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{60FF0D74-8F9C-4552-A2F1-ED4ECD834903}" name="Year(s)"/>
-    <tableColumn id="3" xr3:uid="{BC0C6D42-DC5F-4FFA-9729-00E7AB00058F}" name="Date Last Accessed" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{8FD95ADE-01A2-4ACA-B768-E71CE9CDB424}" name="Source" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{33CBEF15-9BC0-4D4B-9173-8EC128E3881C}" name="Publicly Available"/>
-    <tableColumn id="6" xr3:uid="{7220B94F-00EF-4A7F-B244-7D230476549E}" name="Total Number of Participants"/>
-    <tableColumn id="7" xr3:uid="{4C69384A-EADB-4259-BA31-F2A826478CEF}" name="Cancer Incidence" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{50952C84-1E33-4375-B34F-ABD56E90A66E}" name="Smoking Status" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{8A83B153-EFF8-4762-AB0E-F097D3D2EEE5}" name="Alcohol Usage" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{E08E0576-A282-4612-B6B2-1743EC5098BD}" name="BMI" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{FC4CF880-F6AC-4B08-9A09-537AC7D53D62}" name="Physical Activity" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{330DABF8-CDB0-42BA-99B1-EDAADCD359C6}" name="Daily Diet" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{19F95E98-3538-4B7E-81F9-BDED2C5F55CB}" name="Dataset" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{60FF0D74-8F9C-4552-A2F1-ED4ECD834903}" name="Year(s)" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{BC0C6D42-DC5F-4FFA-9729-00E7AB00058F}" name="Date Last Accessed" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{8FD95ADE-01A2-4ACA-B768-E71CE9CDB424}" name="Source" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{33CBEF15-9BC0-4D4B-9173-8EC128E3881C}" name="Publicly Available" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{7220B94F-00EF-4A7F-B244-7D230476549E}" name="Total Number of Participants" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{4C69384A-EADB-4259-BA31-F2A826478CEF}" name="Cancer Incidence" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{50952C84-1E33-4375-B34F-ABD56E90A66E}" name="Smoking Status" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{8A83B153-EFF8-4762-AB0E-F097D3D2EEE5}" name="Alcohol Usage" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{E08E0576-A282-4612-B6B2-1743EC5098BD}" name="BMI" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{FC4CF880-F6AC-4B08-9A09-537AC7D53D62}" name="Physical Activity" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{330DABF8-CDB0-42BA-99B1-EDAADCD359C6}" name="Daily Diet" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -581,599 +749,595 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E06746-C8FC-437E-B536-154AE66650B7}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" customWidth="1"/>
+    <col min="7" max="12" width="9.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>45754</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
         <v>1995</v>
       </c>
-      <c r="C3" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3">
+      <c r="C3" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4">
         <v>19788</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4">
         <v>1996</v>
       </c>
-      <c r="C4" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4">
+      <c r="C4" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="4">
         <v>20328</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="5"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
         <v>1997</v>
       </c>
-      <c r="C5" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5">
+      <c r="C5" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4">
         <v>15546</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
         <v>1998</v>
       </c>
-      <c r="C6" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6">
+      <c r="C6" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4">
         <v>19654</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
         <v>1999</v>
       </c>
-      <c r="C7" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7">
+      <c r="C7" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4">
         <v>9640</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
         <v>2000</v>
       </c>
-      <c r="C8" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8">
+      <c r="C8" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4">
         <v>12413</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4">
         <v>2001</v>
       </c>
-      <c r="C9" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9">
+      <c r="C9" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4">
         <v>19640</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="5"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4">
         <v>2002</v>
       </c>
-      <c r="C10" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10">
+      <c r="C10" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="4">
         <v>18396</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
         <v>2003</v>
       </c>
-      <c r="C11" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11">
+      <c r="C11" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="4">
         <v>18553</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4">
         <v>2004</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="5">
         <v>45596</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12">
+      <c r="D12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="4">
         <v>8354</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4">
         <v>2005</v>
       </c>
-      <c r="C13" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13">
+      <c r="C13" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="4">
         <v>13297</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4">
         <v>2006</v>
       </c>
-      <c r="C14" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14">
+      <c r="C14" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="4">
         <v>21399</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="5"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4">
         <v>2007</v>
       </c>
-      <c r="C15" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15">
+      <c r="C15" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="4">
         <v>14386</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4">
         <v>2008</v>
       </c>
-      <c r="C16" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16">
+      <c r="C16" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="4">
         <v>22619</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4">
         <v>2009</v>
       </c>
-      <c r="C17" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17">
+      <c r="C17" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="4">
         <v>8602</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4">
         <v>2010</v>
       </c>
-      <c r="C18" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18">
+      <c r="C18" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="4">
         <v>14112</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="4"/>
       <c r="H18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4">
         <v>2011</v>
       </c>
-      <c r="C19" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19">
+      <c r="C19" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="4">
         <v>10617</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="4"/>
       <c r="H19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1183,29 +1347,29 @@
       <c r="J19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="4">
         <v>2012</v>
       </c>
-      <c r="C20" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20">
+      <c r="C20" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="4">
         <v>10333</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1218,28 +1382,28 @@
       <c r="K20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="5"/>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21">
+      <c r="A21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="4">
         <v>2013</v>
       </c>
-      <c r="C21" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21">
+      <c r="C21" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="4">
         <v>10980</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
         <v>17</v>
       </c>
@@ -1249,29 +1413,29 @@
       <c r="J21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="4">
         <v>2014</v>
       </c>
-      <c r="C22" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22">
+      <c r="C22" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="4">
         <v>10080</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G22" s="4"/>
       <c r="H22" s="4" t="s">
         <v>17</v>
       </c>
@@ -1281,29 +1445,29 @@
       <c r="J22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
+      <c r="A23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4">
         <v>2015</v>
       </c>
-      <c r="C23" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23">
+      <c r="C23" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="4">
         <v>13748</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
         <v>17</v>
       </c>
@@ -1313,29 +1477,29 @@
       <c r="J23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4">
         <v>2016</v>
       </c>
-      <c r="C24" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24">
+      <c r="C24" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="4">
         <v>10067</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="4"/>
       <c r="H24" s="4" t="s">
         <v>17</v>
       </c>
@@ -1348,28 +1512,28 @@
       <c r="K24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25">
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="4">
         <v>2017</v>
       </c>
-      <c r="C25" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25">
+      <c r="C25" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="4">
         <v>9982</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="G25" s="4"/>
       <c r="H25" s="4" t="s">
         <v>17</v>
       </c>
@@ -1379,29 +1543,29 @@
       <c r="J25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26">
+      <c r="A26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="4">
         <v>2018</v>
       </c>
-      <c r="C26" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26">
+      <c r="C26" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="4">
         <v>10250</v>
       </c>
-      <c r="G26" s="5"/>
+      <c r="G26" s="4"/>
       <c r="H26" s="4" t="s">
         <v>17</v>
       </c>
@@ -1411,29 +1575,29 @@
       <c r="J26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27">
+      <c r="A27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4">
         <v>2019</v>
       </c>
-      <c r="C27" s="1">
-        <v>45595</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27">
+      <c r="C27" s="5">
+        <v>45595</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="4">
         <v>10299</v>
       </c>
-      <c r="G27" s="5"/>
+      <c r="G27" s="4"/>
       <c r="H27" s="4" t="s">
         <v>17</v>
       </c>
@@ -1443,347 +1607,347 @@
       <c r="J27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="4">
         <v>2005</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="5">
         <v>45600</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28">
+      <c r="D28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="4">
         <v>30069</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>2008</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="5">
         <v>45602</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29">
+      <c r="D29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="4">
         <v>1646</v>
       </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
       <c r="L29" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="4">
         <v>2009</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="5">
         <v>45602</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30">
+      <c r="D30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="4">
         <v>1669</v>
       </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
       <c r="L30" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="4">
         <v>2010</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="5">
         <v>45602</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31">
+      <c r="D31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="4">
         <v>1565</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
       <c r="L31" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="4">
         <v>2011</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="5">
         <v>45602</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32">
+      <c r="D32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="4">
         <v>1948</v>
       </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
       <c r="L32" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="4">
         <v>2012</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="5">
         <v>45602</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33">
+      <c r="D33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="4">
         <v>1197</v>
       </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
       <c r="L33" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="4">
         <v>2013</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="5">
         <v>45602</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34">
+      <c r="D34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="4">
         <v>1349</v>
       </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
       <c r="L34" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="4">
         <v>2014</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="5">
         <v>45602</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35">
+      <c r="D35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="4">
         <v>1353</v>
       </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
       <c r="L35" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="4">
         <v>2015</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="5">
         <v>45602</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36">
+      <c r="D36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="4">
         <v>1370</v>
       </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
       <c r="L36" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="4">
         <v>2016</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="5">
         <v>45602</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37">
+      <c r="D37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="4">
         <v>1253</v>
       </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
       <c r="L37" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="4">
         <v>2017</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="5">
         <v>45602</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38">
+      <c r="D38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="4">
         <v>1211</v>
       </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
       <c r="L38" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="4">
         <v>2018</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="5">
         <v>45602</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39">
+      <c r="D39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="4">
         <v>1094</v>
       </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
       <c r="L39" s="4" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D76A4A9D-2BCC-4C52-9B81-505C0D7FAF41}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{F48FE71B-4E02-4FC1-8FEA-70FF94DFC972}"/>

</xml_diff>